<commit_message>
Antes de Generales Mantenedor de Parametros
</commit_message>
<xml_diff>
--- a/Documentacion APPs/Documentacion SA - MENUS.xlsx
+++ b/Documentacion APPs/Documentacion SA - MENUS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Parametro" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="91">
   <si>
     <t>nParCodigo</t>
   </si>
@@ -183,9 +183,6 @@
     <t>xajax_Nuevo_Sector();</t>
   </si>
   <si>
-    <t>xajax_Rpt_Sector_Pdf(xajax.getFormValues(FrmPrincipal));(xajax.getFormValues(FrmPrincipal));</t>
-  </si>
-  <si>
     <t>xajax_Nuevo_Productor();</t>
   </si>
   <si>
@@ -232,6 +229,66 @@
   </si>
   <si>
     <t>xajax_Listar_Parcelas();</t>
+  </si>
+  <si>
+    <t>Cosecha</t>
+  </si>
+  <si>
+    <t>xajax_Listar_Cosechas();</t>
+  </si>
+  <si>
+    <t>xajax_Nuevo_Cosecha();</t>
+  </si>
+  <si>
+    <t>xajax_Listar_Cosechas(0,15,1,1);</t>
+  </si>
+  <si>
+    <t>xajax_Editar_Cosecha(xajax.getFormValues(FrmPrincipal));</t>
+  </si>
+  <si>
+    <t>xajax_Eliminar_Cosecha(xajax.getFormValues(FrmPrincipal));</t>
+  </si>
+  <si>
+    <t>xajax_Rpt_Cosecha_Pdf(xajax.getFormValues(FrmPrincipal));</t>
+  </si>
+  <si>
+    <t>xajax_Configurar_Parametro(2007);</t>
+  </si>
+  <si>
+    <t>PRODUCTOS</t>
+  </si>
+  <si>
+    <t>Producto</t>
+  </si>
+  <si>
+    <t>PRODUCTO</t>
+  </si>
+  <si>
+    <t>xajax_Nuevo_Parametro();</t>
+  </si>
+  <si>
+    <t>xajax_Editar_Parametro(xajax.getFormValues(FrmPrincipal));</t>
+  </si>
+  <si>
+    <t>xajax_Eliminar_Parametro(xajax.getFormValues(FrmPrincipal));</t>
+  </si>
+  <si>
+    <t>xajax_Rpt_Parametro_Pdf(xajax.getFormValues(FrmPrincipal));</t>
+  </si>
+  <si>
+    <t>xajax_Rpt_Sector_Pdf(xajax.getFormValues(FrmPrincipal));</t>
+  </si>
+  <si>
+    <t>Prueba</t>
+  </si>
+  <si>
+    <t>xajax_Configurar_Parametro(2006);</t>
+  </si>
+  <si>
+    <t>PRUEBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRUEBA </t>
   </si>
 </sst>
 </file>
@@ -586,11 +643,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H34"/>
+  <dimension ref="B1:H59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="B22:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,66 +1097,63 @@
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22">
-        <v>1002</v>
-      </c>
-      <c r="C22">
-        <v>5000</v>
-      </c>
-      <c r="D22">
-        <v>1002</v>
-      </c>
-      <c r="E22" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" t="s">
-        <v>48</v>
-      </c>
-      <c r="G22">
+      <c r="B22" s="2">
+        <v>100104</v>
+      </c>
+      <c r="C22" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D22" s="2">
+        <v>100104</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G22" s="2">
         <v>1</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23">
-        <v>100201</v>
+        <v>10010401</v>
       </c>
       <c r="C23">
-        <v>5000</v>
+        <v>5001</v>
       </c>
       <c r="D23">
-        <v>100201</v>
+        <v>10010401</v>
       </c>
       <c r="E23" t="s">
-        <v>49</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
+      </c>
+      <c r="F23" t="s">
+        <v>16</v>
       </c>
       <c r="G23">
         <v>1</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>10020101</v>
+        <v>10010402</v>
       </c>
       <c r="C24">
         <v>5001</v>
       </c>
       <c r="D24">
-        <v>10020101</v>
+        <v>10010402</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
-      </c>
-      <c r="F24" t="s">
-        <v>16</v>
+        <v>41</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -1107,19 +1161,19 @@
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25">
-        <v>10020102</v>
+        <v>10010403</v>
       </c>
       <c r="C25">
         <v>5001</v>
       </c>
       <c r="D25">
-        <v>10020102</v>
+        <v>10010403</v>
       </c>
       <c r="E25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F25" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -1127,19 +1181,19 @@
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26">
-        <v>10020103</v>
+        <v>10010404</v>
       </c>
       <c r="C26">
         <v>5001</v>
       </c>
       <c r="D26">
-        <v>10020103</v>
+        <v>10010404</v>
       </c>
       <c r="E26" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F26" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -1147,82 +1201,82 @@
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27">
-        <v>10020104</v>
+        <v>10010405</v>
       </c>
       <c r="C27">
         <v>5001</v>
       </c>
       <c r="D27">
-        <v>10020104</v>
+        <v>10010405</v>
       </c>
       <c r="E27" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F27" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="G27">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28">
-        <v>10020105</v>
-      </c>
-      <c r="C28">
-        <v>5001</v>
-      </c>
-      <c r="D28">
-        <v>10020105</v>
-      </c>
-      <c r="E28" t="s">
-        <v>44</v>
-      </c>
-      <c r="F28" t="s">
-        <v>32</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
+      <c r="B28" s="2">
+        <v>100105</v>
+      </c>
+      <c r="C28" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D28" s="2">
+        <v>100105</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28" s="2">
+        <v>1</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29">
-        <v>100202</v>
+        <v>10010501</v>
       </c>
       <c r="C29">
-        <v>5000</v>
+        <v>5001</v>
       </c>
       <c r="D29">
-        <v>100202</v>
+        <v>10010501</v>
       </c>
       <c r="E29" t="s">
-        <v>71</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>65</v>
+        <v>40</v>
+      </c>
+      <c r="F29" t="s">
+        <v>16</v>
       </c>
       <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>65</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30">
-        <v>10020201</v>
+        <v>10010502</v>
       </c>
       <c r="C30">
         <v>5001</v>
       </c>
       <c r="D30">
-        <v>10020201</v>
+        <v>10010502</v>
       </c>
       <c r="E30" t="s">
-        <v>40</v>
-      </c>
-      <c r="F30" t="s">
-        <v>16</v>
+        <v>41</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -1230,19 +1284,19 @@
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31">
-        <v>10020202</v>
+        <v>10010503</v>
       </c>
       <c r="C31">
         <v>5001</v>
       </c>
       <c r="D31">
-        <v>10020202</v>
+        <v>10010503</v>
       </c>
       <c r="E31" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -1250,61 +1304,433 @@
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32">
+        <v>10010504</v>
+      </c>
+      <c r="C32">
+        <v>5001</v>
+      </c>
+      <c r="D32">
+        <v>10010504</v>
+      </c>
+      <c r="E32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>10010505</v>
+      </c>
+      <c r="C33">
+        <v>5001</v>
+      </c>
+      <c r="D33">
+        <v>10010505</v>
+      </c>
+      <c r="E33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" t="s">
+        <v>32</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>1002</v>
+      </c>
+      <c r="C41">
+        <v>5000</v>
+      </c>
+      <c r="D41">
+        <v>1002</v>
+      </c>
+      <c r="E41" t="s">
+        <v>47</v>
+      </c>
+      <c r="F41" t="s">
+        <v>48</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>100201</v>
+      </c>
+      <c r="C42">
+        <v>5000</v>
+      </c>
+      <c r="D42">
+        <v>100201</v>
+      </c>
+      <c r="E42" t="s">
+        <v>49</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>10020101</v>
+      </c>
+      <c r="C43">
+        <v>5001</v>
+      </c>
+      <c r="D43">
+        <v>10020101</v>
+      </c>
+      <c r="E43" t="s">
+        <v>40</v>
+      </c>
+      <c r="F43" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>10020102</v>
+      </c>
+      <c r="C44">
+        <v>5001</v>
+      </c>
+      <c r="D44">
+        <v>10020102</v>
+      </c>
+      <c r="E44" t="s">
+        <v>41</v>
+      </c>
+      <c r="F44" t="s">
+        <v>17</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>10020103</v>
+      </c>
+      <c r="C45">
+        <v>5001</v>
+      </c>
+      <c r="D45">
+        <v>10020103</v>
+      </c>
+      <c r="E45" t="s">
+        <v>42</v>
+      </c>
+      <c r="F45" t="s">
+        <v>18</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>10020104</v>
+      </c>
+      <c r="C46">
+        <v>5001</v>
+      </c>
+      <c r="D46">
+        <v>10020104</v>
+      </c>
+      <c r="E46" t="s">
+        <v>43</v>
+      </c>
+      <c r="F46" t="s">
+        <v>19</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>10020105</v>
+      </c>
+      <c r="C47">
+        <v>5001</v>
+      </c>
+      <c r="D47">
+        <v>10020105</v>
+      </c>
+      <c r="E47" t="s">
+        <v>44</v>
+      </c>
+      <c r="F47" t="s">
+        <v>32</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>100202</v>
+      </c>
+      <c r="C48">
+        <v>5000</v>
+      </c>
+      <c r="D48">
+        <v>100202</v>
+      </c>
+      <c r="E48" t="s">
+        <v>70</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>10020201</v>
+      </c>
+      <c r="C49">
+        <v>5001</v>
+      </c>
+      <c r="D49">
+        <v>10020201</v>
+      </c>
+      <c r="E49" t="s">
+        <v>40</v>
+      </c>
+      <c r="F49" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>10020202</v>
+      </c>
+      <c r="C50">
+        <v>5001</v>
+      </c>
+      <c r="D50">
+        <v>10020202</v>
+      </c>
+      <c r="E50" t="s">
+        <v>41</v>
+      </c>
+      <c r="F50" t="s">
+        <v>17</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51">
         <v>10020203</v>
       </c>
-      <c r="C32">
-        <v>5001</v>
-      </c>
-      <c r="D32">
+      <c r="C51">
+        <v>5001</v>
+      </c>
+      <c r="D51">
         <v>10020203</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E51" t="s">
         <v>42</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F51" t="s">
         <v>18</v>
       </c>
-      <c r="G32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33">
+      <c r="G51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52">
         <v>10020204</v>
       </c>
-      <c r="C33">
-        <v>5001</v>
-      </c>
-      <c r="D33">
+      <c r="C52">
+        <v>5001</v>
+      </c>
+      <c r="D52">
         <v>10020204</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E52" t="s">
         <v>43</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F52" t="s">
         <v>19</v>
       </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34">
+      <c r="G52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53">
         <v>10020205</v>
       </c>
-      <c r="C34">
-        <v>5001</v>
-      </c>
-      <c r="D34">
+      <c r="C53">
+        <v>5001</v>
+      </c>
+      <c r="D53">
         <v>10020205</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E53" t="s">
         <v>44</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F53" t="s">
         <v>32</v>
       </c>
-      <c r="G34">
+      <c r="G53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>100203</v>
+      </c>
+      <c r="C54">
+        <v>5000</v>
+      </c>
+      <c r="D54">
+        <v>100203</v>
+      </c>
+      <c r="E54" t="s">
+        <v>72</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>10020301</v>
+      </c>
+      <c r="C55">
+        <v>5001</v>
+      </c>
+      <c r="D55">
+        <v>10020301</v>
+      </c>
+      <c r="E55" t="s">
+        <v>40</v>
+      </c>
+      <c r="F55" t="s">
+        <v>16</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>10020302</v>
+      </c>
+      <c r="C56">
+        <v>5001</v>
+      </c>
+      <c r="D56">
+        <v>10020302</v>
+      </c>
+      <c r="E56" t="s">
+        <v>41</v>
+      </c>
+      <c r="F56" t="s">
+        <v>17</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>10020303</v>
+      </c>
+      <c r="C57">
+        <v>5001</v>
+      </c>
+      <c r="D57">
+        <v>10020303</v>
+      </c>
+      <c r="E57" t="s">
+        <v>42</v>
+      </c>
+      <c r="F57" t="s">
+        <v>18</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>10020304</v>
+      </c>
+      <c r="C58">
+        <v>5001</v>
+      </c>
+      <c r="D58">
+        <v>10020304</v>
+      </c>
+      <c r="E58" t="s">
+        <v>43</v>
+      </c>
+      <c r="F58" t="s">
+        <v>19</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>10020305</v>
+      </c>
+      <c r="C59">
+        <v>5001</v>
+      </c>
+      <c r="D59">
+        <v>10020305</v>
+      </c>
+      <c r="E59" t="s">
+        <v>44</v>
+      </c>
+      <c r="F59" t="s">
+        <v>32</v>
+      </c>
+      <c r="G59">
         <v>1</v>
       </c>
     </row>
@@ -1316,11 +1742,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H29"/>
+  <dimension ref="B1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G29" sqref="B20:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1329,7 +1755,7 @@
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="92.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1476,7 +1902,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -1656,50 +2082,50 @@
         <v>5001</v>
       </c>
       <c r="F19" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <v>100201</v>
-      </c>
-      <c r="C20">
-        <v>5000</v>
-      </c>
-      <c r="D20">
-        <v>10020101</v>
-      </c>
-      <c r="E20">
-        <v>5001</v>
-      </c>
-      <c r="F20" t="s">
-        <v>56</v>
-      </c>
-      <c r="G20">
+      <c r="B20" s="2">
+        <v>100104</v>
+      </c>
+      <c r="C20" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D20" s="2">
+        <v>10010401</v>
+      </c>
+      <c r="E20" s="2">
+        <v>5001</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" s="2">
         <v>1</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21">
-        <v>100201</v>
+        <v>100104</v>
       </c>
       <c r="C21">
         <v>5000</v>
       </c>
       <c r="D21">
-        <v>10020102</v>
+        <v>10010402</v>
       </c>
       <c r="E21">
         <v>5001</v>
       </c>
-      <c r="F21" t="s">
-        <v>57</v>
+      <c r="F21" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1707,19 +2133,19 @@
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>100201</v>
+        <v>100104</v>
       </c>
       <c r="C22">
         <v>5000</v>
       </c>
       <c r="D22">
-        <v>10020103</v>
+        <v>10010403</v>
       </c>
       <c r="E22">
         <v>5001</v>
       </c>
       <c r="F22" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -1727,19 +2153,19 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23">
-        <v>100201</v>
+        <v>100104</v>
       </c>
       <c r="C23">
         <v>5000</v>
       </c>
       <c r="D23">
-        <v>10020104</v>
+        <v>10010404</v>
       </c>
       <c r="E23">
         <v>5001</v>
       </c>
       <c r="F23" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1747,139 +2173,449 @@
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24">
+        <v>100104</v>
+      </c>
+      <c r="C24">
+        <v>5000</v>
+      </c>
+      <c r="D24">
+        <v>10010405</v>
+      </c>
+      <c r="E24">
+        <v>5001</v>
+      </c>
+      <c r="F24" t="s">
+        <v>85</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="2">
+        <v>100105</v>
+      </c>
+      <c r="C25" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D25" s="2">
+        <v>10010501</v>
+      </c>
+      <c r="E25" s="2">
+        <v>5001</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G25" s="2">
+        <v>1</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="2">
+        <v>100105</v>
+      </c>
+      <c r="C26">
+        <v>5000</v>
+      </c>
+      <c r="D26">
+        <v>10010502</v>
+      </c>
+      <c r="E26">
+        <v>5001</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="2">
+        <v>100105</v>
+      </c>
+      <c r="C27">
+        <v>5000</v>
+      </c>
+      <c r="D27">
+        <v>10010503</v>
+      </c>
+      <c r="E27">
+        <v>5001</v>
+      </c>
+      <c r="F27" t="s">
+        <v>83</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
+        <v>100105</v>
+      </c>
+      <c r="C28">
+        <v>5000</v>
+      </c>
+      <c r="D28">
+        <v>10010504</v>
+      </c>
+      <c r="E28">
+        <v>5001</v>
+      </c>
+      <c r="F28" t="s">
+        <v>84</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="2">
+        <v>100105</v>
+      </c>
+      <c r="C29">
+        <v>5000</v>
+      </c>
+      <c r="D29">
+        <v>10010505</v>
+      </c>
+      <c r="E29">
+        <v>5001</v>
+      </c>
+      <c r="F29" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38">
         <v>100201</v>
       </c>
-      <c r="C24">
-        <v>5000</v>
-      </c>
-      <c r="D24">
+      <c r="C38">
+        <v>5000</v>
+      </c>
+      <c r="D38">
+        <v>10020101</v>
+      </c>
+      <c r="E38">
+        <v>5001</v>
+      </c>
+      <c r="F38" t="s">
+        <v>55</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>100201</v>
+      </c>
+      <c r="C39">
+        <v>5000</v>
+      </c>
+      <c r="D39">
+        <v>10020102</v>
+      </c>
+      <c r="E39">
+        <v>5001</v>
+      </c>
+      <c r="F39" t="s">
+        <v>56</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>100201</v>
+      </c>
+      <c r="C40">
+        <v>5000</v>
+      </c>
+      <c r="D40">
+        <v>10020103</v>
+      </c>
+      <c r="E40">
+        <v>5001</v>
+      </c>
+      <c r="F40" t="s">
+        <v>57</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>100201</v>
+      </c>
+      <c r="C41">
+        <v>5000</v>
+      </c>
+      <c r="D41">
+        <v>10020104</v>
+      </c>
+      <c r="E41">
+        <v>5001</v>
+      </c>
+      <c r="F41" t="s">
+        <v>58</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>100201</v>
+      </c>
+      <c r="C42">
+        <v>5000</v>
+      </c>
+      <c r="D42">
         <v>10020105</v>
       </c>
-      <c r="E24">
-        <v>5001</v>
-      </c>
-      <c r="F24" t="s">
-        <v>60</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25">
+      <c r="E42">
+        <v>5001</v>
+      </c>
+      <c r="F42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43">
         <v>100202</v>
       </c>
-      <c r="C25">
-        <v>5000</v>
-      </c>
-      <c r="D25">
+      <c r="C43">
+        <v>5000</v>
+      </c>
+      <c r="D43">
         <v>10020201</v>
       </c>
-      <c r="E25">
-        <v>5001</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="E43">
+        <v>5001</v>
+      </c>
+      <c r="F43" t="s">
+        <v>65</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>100202</v>
+      </c>
+      <c r="C44">
+        <v>5000</v>
+      </c>
+      <c r="D44">
+        <v>10020202</v>
+      </c>
+      <c r="E44">
+        <v>5001</v>
+      </c>
+      <c r="F44" t="s">
         <v>66</v>
       </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26">
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45">
         <v>100202</v>
       </c>
-      <c r="C26">
-        <v>5000</v>
-      </c>
-      <c r="D26">
-        <v>10020202</v>
-      </c>
-      <c r="E26">
-        <v>5001</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="C45">
+        <v>5000</v>
+      </c>
+      <c r="D45">
+        <v>10020203</v>
+      </c>
+      <c r="E45">
+        <v>5001</v>
+      </c>
+      <c r="F45" t="s">
         <v>67</v>
       </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27">
+      <c r="G45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46">
         <v>100202</v>
       </c>
-      <c r="C27">
-        <v>5000</v>
-      </c>
-      <c r="D27">
-        <v>10020203</v>
-      </c>
-      <c r="E27">
-        <v>5001</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="C46">
+        <v>5000</v>
+      </c>
+      <c r="D46">
+        <v>10020204</v>
+      </c>
+      <c r="E46">
+        <v>5001</v>
+      </c>
+      <c r="F46" t="s">
         <v>68</v>
       </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28">
+      <c r="G46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47">
         <v>100202</v>
       </c>
-      <c r="C28">
-        <v>5000</v>
-      </c>
-      <c r="D28">
-        <v>10020204</v>
-      </c>
-      <c r="E28">
-        <v>5001</v>
-      </c>
-      <c r="F28" t="s">
+      <c r="C47">
+        <v>5000</v>
+      </c>
+      <c r="D47">
+        <v>10020205</v>
+      </c>
+      <c r="E47">
+        <v>5001</v>
+      </c>
+      <c r="F47" t="s">
         <v>69</v>
       </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29">
-        <v>100202</v>
-      </c>
-      <c r="C29">
-        <v>5000</v>
-      </c>
-      <c r="D29">
-        <v>10020205</v>
-      </c>
-      <c r="E29">
-        <v>5001</v>
-      </c>
-      <c r="F29" t="s">
-        <v>70</v>
-      </c>
-      <c r="G29">
+      <c r="G47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="2">
+        <v>100203</v>
+      </c>
+      <c r="C48" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D48" s="2">
+        <v>10020301</v>
+      </c>
+      <c r="E48" s="2">
+        <v>5001</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G48" s="2">
+        <v>1</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>100203</v>
+      </c>
+      <c r="C49">
+        <v>5000</v>
+      </c>
+      <c r="D49">
+        <v>10020302</v>
+      </c>
+      <c r="E49">
+        <v>5001</v>
+      </c>
+      <c r="F49" t="s">
+        <v>74</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>100203</v>
+      </c>
+      <c r="C50">
+        <v>5000</v>
+      </c>
+      <c r="D50">
+        <v>10020303</v>
+      </c>
+      <c r="E50">
+        <v>5001</v>
+      </c>
+      <c r="F50" t="s">
+        <v>75</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>100203</v>
+      </c>
+      <c r="C51">
+        <v>5000</v>
+      </c>
+      <c r="D51">
+        <v>10020304</v>
+      </c>
+      <c r="E51">
+        <v>5001</v>
+      </c>
+      <c r="F51" t="s">
+        <v>76</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>100203</v>
+      </c>
+      <c r="C52">
+        <v>5000</v>
+      </c>
+      <c r="D52">
+        <v>10020305</v>
+      </c>
+      <c r="E52">
+        <v>5001</v>
+      </c>
+      <c r="F52" t="s">
+        <v>77</v>
+      </c>
+      <c r="G52">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I34"/>
+  <dimension ref="B1:I62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H34" sqref="B29:H34"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H33" sqref="B22:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1939,7 +2675,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
@@ -2106,7 +2842,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
@@ -2379,297 +3115,727 @@
         <v>5000</v>
       </c>
       <c r="F22" s="2">
+        <v>100104</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2">
+        <v>1</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>5001</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>5001</v>
+      </c>
+      <c r="F23">
+        <v>10010401</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>5001</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>5001</v>
+      </c>
+      <c r="F24">
+        <v>10010402</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>5001</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>5001</v>
+      </c>
+      <c r="F25">
+        <v>10010403</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>5001</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>5001</v>
+      </c>
+      <c r="F26">
+        <v>10010404</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>5001</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>5001</v>
+      </c>
+      <c r="F27">
+        <v>10010405</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2">
+        <v>10</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1</v>
+      </c>
+      <c r="E28" s="2">
+        <v>5000</v>
+      </c>
+      <c r="F28" s="2">
+        <v>100105</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2">
+        <v>1</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>5001</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>5001</v>
+      </c>
+      <c r="F29">
+        <v>10010501</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>5001</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>5001</v>
+      </c>
+      <c r="F30">
+        <v>10010502</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>5001</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>5001</v>
+      </c>
+      <c r="F31">
+        <v>10010503</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>5001</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>5001</v>
+      </c>
+      <c r="F32">
+        <v>10010504</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>5001</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>5001</v>
+      </c>
+      <c r="F33">
+        <v>10010505</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="2">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2">
+        <v>10</v>
+      </c>
+      <c r="D44" s="2">
+        <v>1</v>
+      </c>
+      <c r="E44" s="2">
+        <v>5000</v>
+      </c>
+      <c r="F44" s="2">
         <v>1002</v>
       </c>
-      <c r="G22" s="2">
-        <v>0</v>
-      </c>
-      <c r="H22" s="2">
-        <v>1</v>
-      </c>
-      <c r="I22" s="2" t="s">
+      <c r="G44" s="2">
+        <v>0</v>
+      </c>
+      <c r="H44" s="2">
+        <v>1</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="2">
+        <v>1</v>
+      </c>
+      <c r="C45" s="2">
+        <v>10</v>
+      </c>
+      <c r="D45" s="2">
+        <v>1</v>
+      </c>
+      <c r="E45" s="2">
+        <v>5000</v>
+      </c>
+      <c r="F45" s="2">
+        <v>100201</v>
+      </c>
+      <c r="G45" s="2">
+        <v>0</v>
+      </c>
+      <c r="H45" s="2">
+        <v>1</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>5001</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>5001</v>
+      </c>
+      <c r="F46">
+        <v>10020101</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>5001</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>5001</v>
+      </c>
+      <c r="F47">
+        <v>10020102</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>5001</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>5001</v>
+      </c>
+      <c r="F48">
+        <v>10020103</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>5001</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>5001</v>
+      </c>
+      <c r="F49">
+        <v>10020104</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>5001</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>5001</v>
+      </c>
+      <c r="F50">
+        <v>10020105</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="2">
+        <v>1</v>
+      </c>
+      <c r="C51" s="2">
+        <v>10</v>
+      </c>
+      <c r="D51" s="2">
+        <v>1</v>
+      </c>
+      <c r="E51" s="2">
+        <v>5000</v>
+      </c>
+      <c r="F51" s="2">
+        <v>100202</v>
+      </c>
+      <c r="G51" s="2">
+        <v>0</v>
+      </c>
+      <c r="H51" s="2">
+        <v>1</v>
+      </c>
+      <c r="I51" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="2">
-        <v>1</v>
-      </c>
-      <c r="C23" s="2">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>5001</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>5001</v>
+      </c>
+      <c r="F52">
+        <v>10020201</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>5001</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>5001</v>
+      </c>
+      <c r="F53">
+        <v>10020202</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>5001</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>5001</v>
+      </c>
+      <c r="F54">
+        <v>10020203</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>5001</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>5001</v>
+      </c>
+      <c r="F55">
+        <v>10020204</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>5001</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>5001</v>
+      </c>
+      <c r="F56">
+        <v>10020205</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="2">
+        <v>1</v>
+      </c>
+      <c r="C57" s="2">
         <v>10</v>
       </c>
-      <c r="D23" s="2">
-        <v>1</v>
-      </c>
-      <c r="E23" s="2">
-        <v>5000</v>
-      </c>
-      <c r="F23" s="2">
-        <v>100201</v>
-      </c>
-      <c r="G23" s="2">
-        <v>0</v>
-      </c>
-      <c r="H23" s="2">
-        <v>1</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <v>5001</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>5001</v>
-      </c>
-      <c r="F24">
-        <v>10020101</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <v>5001</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>5001</v>
-      </c>
-      <c r="F25">
-        <v>10020102</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>5001</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26">
-        <v>5001</v>
-      </c>
-      <c r="F26">
-        <v>10020103</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <v>5001</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>5001</v>
-      </c>
-      <c r="F27">
-        <v>10020104</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>5001</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28">
-        <v>5001</v>
-      </c>
-      <c r="F28">
-        <v>10020105</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="2">
-        <v>1</v>
-      </c>
-      <c r="C29" s="2">
-        <v>10</v>
-      </c>
-      <c r="D29" s="2">
-        <v>1</v>
-      </c>
-      <c r="E29" s="2">
-        <v>5000</v>
-      </c>
-      <c r="F29" s="2">
-        <v>100202</v>
-      </c>
-      <c r="G29" s="2">
-        <v>0</v>
-      </c>
-      <c r="H29" s="2">
-        <v>1</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>5001</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30">
-        <v>5001</v>
-      </c>
-      <c r="F30">
-        <v>10020201</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31">
-        <v>5001</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <v>5001</v>
-      </c>
-      <c r="F31">
-        <v>10020202</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32">
-        <v>5001</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32">
-        <v>5001</v>
-      </c>
-      <c r="F32">
-        <v>10020203</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33">
-        <v>5001</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33">
-        <v>5001</v>
-      </c>
-      <c r="F33">
-        <v>10020204</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34">
-        <v>5001</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34">
-        <v>5001</v>
-      </c>
-      <c r="F34">
-        <v>10020205</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34">
+      <c r="D57" s="2">
+        <v>1</v>
+      </c>
+      <c r="E57" s="2">
+        <v>5000</v>
+      </c>
+      <c r="F57" s="2">
+        <v>100203</v>
+      </c>
+      <c r="G57" s="2">
+        <v>0</v>
+      </c>
+      <c r="H57" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>5001</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>5001</v>
+      </c>
+      <c r="F58">
+        <v>10020301</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>5001</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>5001</v>
+      </c>
+      <c r="F59">
+        <v>10020302</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>5001</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>5001</v>
+      </c>
+      <c r="F60">
+        <v>10020303</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61">
+        <v>5001</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>5001</v>
+      </c>
+      <c r="F61">
+        <v>10020304</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>5001</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>5001</v>
+      </c>
+      <c r="F62">
+        <v>10020305</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Hasta Mantenedor de Parametro global
</commit_message>
<xml_diff>
--- a/Documentacion APPs/Documentacion SA - MENUS.xlsx
+++ b/Documentacion APPs/Documentacion SA - MENUS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Parametro" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="87">
   <si>
     <t>nParCodigo</t>
   </si>
@@ -277,18 +277,6 @@
   </si>
   <si>
     <t>xajax_Rpt_Sector_Pdf(xajax.getFormValues(FrmPrincipal));</t>
-  </si>
-  <si>
-    <t>Prueba</t>
-  </si>
-  <si>
-    <t>xajax_Configurar_Parametro(2006);</t>
-  </si>
-  <si>
-    <t>PRUEBA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRUEBA </t>
   </si>
 </sst>
 </file>
@@ -645,9 +633,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="B22:G33"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,127 +1208,15 @@
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="2">
-        <v>100105</v>
-      </c>
-      <c r="C28" s="2">
-        <v>5000</v>
-      </c>
-      <c r="D28" s="2">
-        <v>100105</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G28" s="2">
-        <v>1</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29">
-        <v>10010501</v>
-      </c>
-      <c r="C29">
-        <v>5001</v>
-      </c>
-      <c r="D29">
-        <v>10010501</v>
-      </c>
-      <c r="E29" t="s">
-        <v>40</v>
-      </c>
-      <c r="F29" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30">
-        <v>10010502</v>
-      </c>
-      <c r="C30">
-        <v>5001</v>
-      </c>
-      <c r="D30">
-        <v>10010502</v>
-      </c>
-      <c r="E30" t="s">
-        <v>41</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31">
-        <v>10010503</v>
-      </c>
-      <c r="C31">
-        <v>5001</v>
-      </c>
-      <c r="D31">
-        <v>10010503</v>
-      </c>
-      <c r="E31" t="s">
-        <v>42</v>
-      </c>
-      <c r="F31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32">
-        <v>10010504</v>
-      </c>
-      <c r="C32">
-        <v>5001</v>
-      </c>
-      <c r="D32">
-        <v>10010504</v>
-      </c>
-      <c r="E32" t="s">
-        <v>43</v>
-      </c>
-      <c r="F32" t="s">
-        <v>19</v>
-      </c>
-      <c r="G32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33">
-        <v>10010505</v>
-      </c>
-      <c r="C33">
-        <v>5001</v>
-      </c>
-      <c r="D33">
-        <v>10010505</v>
-      </c>
-      <c r="E33" t="s">
-        <v>44</v>
-      </c>
-      <c r="F33" t="s">
-        <v>32</v>
-      </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
+      <c r="F30" s="3"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41">
@@ -1744,9 +1620,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G29" sqref="B20:G29"/>
+      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2192,107 +2068,25 @@
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="2">
-        <v>100105</v>
-      </c>
-      <c r="C25" s="2">
-        <v>5000</v>
-      </c>
-      <c r="D25" s="2">
-        <v>10010501</v>
-      </c>
-      <c r="E25" s="2">
-        <v>5001</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G25" s="2">
-        <v>1</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>89</v>
-      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="2">
-        <v>100105</v>
-      </c>
-      <c r="C26">
-        <v>5000</v>
-      </c>
-      <c r="D26">
-        <v>10010502</v>
-      </c>
-      <c r="E26">
-        <v>5001</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
+      <c r="B26" s="2"/>
+      <c r="F26" s="3"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="2">
-        <v>100105</v>
-      </c>
-      <c r="C27">
-        <v>5000</v>
-      </c>
-      <c r="D27">
-        <v>10010503</v>
-      </c>
-      <c r="E27">
-        <v>5001</v>
-      </c>
-      <c r="F27" t="s">
-        <v>83</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
+      <c r="B27" s="2"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="2">
-        <v>100105</v>
-      </c>
-      <c r="C28">
-        <v>5000</v>
-      </c>
-      <c r="D28">
-        <v>10010504</v>
-      </c>
-      <c r="E28">
-        <v>5001</v>
-      </c>
-      <c r="F28" t="s">
-        <v>84</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
+      <c r="B28" s="2"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="2">
-        <v>100105</v>
-      </c>
-      <c r="C29">
-        <v>5000</v>
-      </c>
-      <c r="D29">
-        <v>10010505</v>
-      </c>
-      <c r="E29">
-        <v>5001</v>
-      </c>
-      <c r="F29" t="s">
-        <v>85</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
+      <c r="B29" s="2"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38">
@@ -2615,7 +2409,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H33" sqref="B22:H33"/>
+      <selection pane="bottomLeft" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3243,146 +3037,19 @@
       </c>
     </row>
     <row r="28" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="2">
-        <v>1</v>
-      </c>
-      <c r="C28" s="2">
-        <v>10</v>
-      </c>
-      <c r="D28" s="2">
-        <v>1</v>
-      </c>
-      <c r="E28" s="2">
-        <v>5000</v>
-      </c>
-      <c r="F28" s="2">
-        <v>100105</v>
-      </c>
-      <c r="G28" s="2">
-        <v>0</v>
-      </c>
-      <c r="H28" s="2">
-        <v>1</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <v>5001</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <v>5001</v>
-      </c>
-      <c r="F29">
-        <v>10010501</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>5001</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30">
-        <v>5001</v>
-      </c>
-      <c r="F30">
-        <v>10010502</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31">
-        <v>5001</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <v>5001</v>
-      </c>
-      <c r="F31">
-        <v>10010503</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32">
-        <v>5001</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32">
-        <v>5001</v>
-      </c>
-      <c r="F32">
-        <v>10010504</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33">
-        <v>5001</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33">
-        <v>5001</v>
-      </c>
-      <c r="F33">
-        <v>10010505</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
-    </row>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Hasta Series - OK
</commit_message>
<xml_diff>
--- a/Documentacion APPs/Documentacion SA - MENUS.xlsx
+++ b/Documentacion APPs/Documentacion SA - MENUS.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Parametro" sheetId="1" r:id="rId1"/>
     <sheet name="ParParametro" sheetId="2" r:id="rId2"/>
     <sheet name="PerUsuAcceso" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="108">
   <si>
     <t>nParCodigo</t>
   </si>
@@ -277,6 +277,69 @@
   </si>
   <si>
     <t>xajax_Rpt_Sector_Pdf(xajax.getFormValues(FrmPrincipal));</t>
+  </si>
+  <si>
+    <t>Maestro Docuemento</t>
+  </si>
+  <si>
+    <t>Comprobante Pago</t>
+  </si>
+  <si>
+    <t>Comprobantes</t>
+  </si>
+  <si>
+    <t>xajax_Configurar_Parametro(1007);</t>
+  </si>
+  <si>
+    <t>Maestro Documento</t>
+  </si>
+  <si>
+    <t>Series</t>
+  </si>
+  <si>
+    <t>xajax_Configurar_Parametro(1008);</t>
+  </si>
+  <si>
+    <t>SERIES</t>
+  </si>
+  <si>
+    <t>COMPROBATES DE PAGO</t>
+  </si>
+  <si>
+    <t>Comprobante Pagos</t>
+  </si>
+  <si>
+    <t>ASIGNAR SERIES</t>
+  </si>
+  <si>
+    <t>Asignar Series</t>
+  </si>
+  <si>
+    <t>xajax_Listar_AsignarSeries(0,20,1,1);</t>
+  </si>
+  <si>
+    <t>xajax_Nuevo_AsignarSerie();</t>
+  </si>
+  <si>
+    <t>xajax_Editar_AsignarSerie(xajax.getFormValues(FrmPrincipal));</t>
+  </si>
+  <si>
+    <t>xajax_Eliminar_AsignarSerie(xajax.getFormValues(FrmPrincipal));</t>
+  </si>
+  <si>
+    <t>xajax_Rpt_AsignarSerie_Pdf(xajax.getFormValues(FrmPrincipal));</t>
+  </si>
+  <si>
+    <t>PUNTOS DE EMISION</t>
+  </si>
+  <si>
+    <t>xajax_Configurar_Parametro(1009);</t>
+  </si>
+  <si>
+    <t>Punto de Emisión</t>
+  </si>
+  <si>
+    <t>PUNTOS DE EMISON</t>
   </si>
 </sst>
 </file>
@@ -631,11 +694,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H59"/>
+  <dimension ref="B1:H74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K31" sqref="K31"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B63" sqref="B63:H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,77 +1271,332 @@
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="B28">
+        <v>1002</v>
+      </c>
+      <c r="C28">
+        <v>5000</v>
+      </c>
+      <c r="D28">
+        <v>1002</v>
+      </c>
+      <c r="E28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" t="s">
+        <v>48</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>100201</v>
+      </c>
+      <c r="C29">
+        <v>5000</v>
+      </c>
+      <c r="D29">
+        <v>100201</v>
+      </c>
+      <c r="E29" t="s">
+        <v>49</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F30" s="3"/>
+      <c r="B30">
+        <v>10020101</v>
+      </c>
+      <c r="C30">
+        <v>5001</v>
+      </c>
+      <c r="D30">
+        <v>10020101</v>
+      </c>
+      <c r="E30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>10020102</v>
+      </c>
+      <c r="C31">
+        <v>5001</v>
+      </c>
+      <c r="D31">
+        <v>10020102</v>
+      </c>
+      <c r="E31" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>10020103</v>
+      </c>
+      <c r="C32">
+        <v>5001</v>
+      </c>
+      <c r="D32">
+        <v>10020103</v>
+      </c>
+      <c r="E32" t="s">
+        <v>42</v>
+      </c>
+      <c r="F32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>10020104</v>
+      </c>
+      <c r="C33">
+        <v>5001</v>
+      </c>
+      <c r="D33">
+        <v>10020104</v>
+      </c>
+      <c r="E33" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>10020105</v>
+      </c>
+      <c r="C34">
+        <v>5001</v>
+      </c>
+      <c r="D34">
+        <v>10020105</v>
+      </c>
+      <c r="E34" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>100202</v>
+      </c>
+      <c r="C35">
+        <v>5000</v>
+      </c>
+      <c r="D35">
+        <v>100202</v>
+      </c>
+      <c r="E35" t="s">
+        <v>70</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>10020201</v>
+      </c>
+      <c r="C36">
+        <v>5001</v>
+      </c>
+      <c r="D36">
+        <v>10020201</v>
+      </c>
+      <c r="E36" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>10020202</v>
+      </c>
+      <c r="C37">
+        <v>5001</v>
+      </c>
+      <c r="D37">
+        <v>10020202</v>
+      </c>
+      <c r="E37" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>10020203</v>
+      </c>
+      <c r="C38">
+        <v>5001</v>
+      </c>
+      <c r="D38">
+        <v>10020203</v>
+      </c>
+      <c r="E38" t="s">
+        <v>42</v>
+      </c>
+      <c r="F38" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>10020204</v>
+      </c>
+      <c r="C39">
+        <v>5001</v>
+      </c>
+      <c r="D39">
+        <v>10020204</v>
+      </c>
+      <c r="E39" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39" t="s">
+        <v>19</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>10020205</v>
+      </c>
+      <c r="C40">
+        <v>5001</v>
+      </c>
+      <c r="D40">
+        <v>10020205</v>
+      </c>
+      <c r="E40" t="s">
+        <v>44</v>
+      </c>
+      <c r="F40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41">
-        <v>1002</v>
+        <v>100203</v>
       </c>
       <c r="C41">
         <v>5000</v>
       </c>
       <c r="D41">
-        <v>1002</v>
+        <v>100203</v>
       </c>
       <c r="E41" t="s">
-        <v>47</v>
-      </c>
-      <c r="F41" t="s">
-        <v>48</v>
+        <v>72</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="G41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42">
-        <v>100201</v>
+        <v>10020301</v>
       </c>
       <c r="C42">
-        <v>5000</v>
+        <v>5001</v>
       </c>
       <c r="D42">
-        <v>100201</v>
+        <v>10020301</v>
       </c>
       <c r="E42" t="s">
-        <v>49</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
+      </c>
+      <c r="F42" t="s">
+        <v>16</v>
       </c>
       <c r="G42">
         <v>1</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43">
-        <v>10020101</v>
+        <v>10020302</v>
       </c>
       <c r="C43">
         <v>5001</v>
       </c>
       <c r="D43">
-        <v>10020101</v>
+        <v>10020302</v>
       </c>
       <c r="E43" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F43" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -1286,19 +1604,19 @@
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44">
-        <v>10020102</v>
+        <v>10020303</v>
       </c>
       <c r="C44">
         <v>5001</v>
       </c>
       <c r="D44">
-        <v>10020102</v>
+        <v>10020303</v>
       </c>
       <c r="E44" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F44" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G44">
         <v>1</v>
@@ -1306,19 +1624,19 @@
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45">
-        <v>10020103</v>
+        <v>10020304</v>
       </c>
       <c r="C45">
         <v>5001</v>
       </c>
       <c r="D45">
-        <v>10020103</v>
+        <v>10020304</v>
       </c>
       <c r="E45" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F45" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G45">
         <v>1</v>
@@ -1326,142 +1644,106 @@
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46">
-        <v>10020104</v>
+        <v>10020305</v>
       </c>
       <c r="C46">
         <v>5001</v>
       </c>
       <c r="D46">
-        <v>10020104</v>
+        <v>10020305</v>
       </c>
       <c r="E46" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F46" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="G46">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47">
-        <v>10020105</v>
-      </c>
-      <c r="C47">
-        <v>5001</v>
-      </c>
-      <c r="D47">
-        <v>10020105</v>
-      </c>
-      <c r="E47" t="s">
-        <v>44</v>
-      </c>
-      <c r="F47" t="s">
-        <v>32</v>
-      </c>
-      <c r="G47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B48">
-        <v>100202</v>
-      </c>
-      <c r="C48">
-        <v>5000</v>
-      </c>
-      <c r="D48">
-        <v>100202</v>
-      </c>
-      <c r="E48" t="s">
-        <v>70</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49">
-        <v>10020201</v>
-      </c>
-      <c r="C49">
-        <v>5001</v>
-      </c>
-      <c r="D49">
-        <v>10020201</v>
-      </c>
-      <c r="E49" t="s">
-        <v>40</v>
-      </c>
-      <c r="F49" t="s">
-        <v>16</v>
-      </c>
-      <c r="G49">
-        <v>1</v>
+      <c r="B49" s="2">
+        <v>1003</v>
+      </c>
+      <c r="C49" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D49" s="2">
+        <v>1003</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G49" s="2">
+        <v>1</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50">
-        <v>10020202</v>
-      </c>
-      <c r="C50">
-        <v>5001</v>
-      </c>
-      <c r="D50">
-        <v>10020202</v>
-      </c>
-      <c r="E50" t="s">
-        <v>41</v>
-      </c>
-      <c r="F50" t="s">
-        <v>17</v>
-      </c>
-      <c r="G50">
-        <v>1</v>
+      <c r="B50" s="2">
+        <v>100301</v>
+      </c>
+      <c r="C50" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D50" s="2">
+        <v>100301</v>
+      </c>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G50" s="2">
+        <v>1</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51">
-        <v>10020203</v>
-      </c>
-      <c r="C51">
-        <v>5001</v>
-      </c>
-      <c r="D51">
-        <v>10020203</v>
-      </c>
-      <c r="E51" t="s">
-        <v>42</v>
-      </c>
-      <c r="F51" t="s">
-        <v>18</v>
-      </c>
-      <c r="G51">
-        <v>1</v>
+      <c r="B51" s="2">
+        <v>10030101</v>
+      </c>
+      <c r="C51" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D51" s="2">
+        <v>10030101</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G51" s="2">
+        <v>1</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52">
-        <v>10020204</v>
+        <v>1003010101</v>
       </c>
       <c r="C52">
         <v>5001</v>
       </c>
       <c r="D52">
-        <v>10020204</v>
+        <v>1003010101</v>
       </c>
       <c r="E52" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F52" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G52">
         <v>1</v>
@@ -1469,19 +1751,19 @@
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53">
-        <v>10020205</v>
+        <v>1003010102</v>
       </c>
       <c r="C53">
         <v>5001</v>
       </c>
       <c r="D53">
-        <v>10020205</v>
+        <v>1003010102</v>
       </c>
       <c r="E53" t="s">
-        <v>44</v>
-      </c>
-      <c r="F53" t="s">
-        <v>32</v>
+        <v>41</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="G53">
         <v>1</v>
@@ -1489,42 +1771,39 @@
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54">
-        <v>100203</v>
+        <v>1003010103</v>
       </c>
       <c r="C54">
-        <v>5000</v>
+        <v>5001</v>
       </c>
       <c r="D54">
-        <v>100203</v>
+        <v>1003010103</v>
       </c>
       <c r="E54" t="s">
-        <v>72</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>71</v>
+        <v>42</v>
+      </c>
+      <c r="F54" t="s">
+        <v>18</v>
       </c>
       <c r="G54">
-        <v>0</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>71</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55">
-        <v>10020301</v>
+        <v>1003010104</v>
       </c>
       <c r="C55">
         <v>5001</v>
       </c>
       <c r="D55">
-        <v>10020301</v>
+        <v>1003010104</v>
       </c>
       <c r="E55" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F55" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G55">
         <v>1</v>
@@ -1532,59 +1811,62 @@
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56">
-        <v>10020302</v>
+        <v>1003010105</v>
       </c>
       <c r="C56">
         <v>5001</v>
       </c>
       <c r="D56">
-        <v>10020302</v>
+        <v>1003010105</v>
       </c>
       <c r="E56" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F56" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="G56">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B57">
-        <v>10020303</v>
-      </c>
-      <c r="C57">
-        <v>5001</v>
-      </c>
-      <c r="D57">
-        <v>10020303</v>
-      </c>
-      <c r="E57" t="s">
-        <v>42</v>
-      </c>
-      <c r="F57" t="s">
-        <v>18</v>
-      </c>
-      <c r="G57">
-        <v>1</v>
+      <c r="B57" s="2">
+        <v>10030102</v>
+      </c>
+      <c r="C57" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D57" s="2">
+        <v>10030102</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G57" s="2">
+        <v>1</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58">
-        <v>10020304</v>
+        <v>1003010201</v>
       </c>
       <c r="C58">
         <v>5001</v>
       </c>
       <c r="D58">
-        <v>10020304</v>
+        <v>1003010201</v>
       </c>
       <c r="E58" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F58" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G58">
         <v>1</v>
@@ -1592,21 +1874,327 @@
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59">
-        <v>10020305</v>
+        <v>1003010202</v>
       </c>
       <c r="C59">
         <v>5001</v>
       </c>
       <c r="D59">
-        <v>10020305</v>
+        <v>1003010202</v>
       </c>
       <c r="E59" t="s">
+        <v>41</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>1003010203</v>
+      </c>
+      <c r="C60">
+        <v>5001</v>
+      </c>
+      <c r="D60">
+        <v>1003010203</v>
+      </c>
+      <c r="E60" t="s">
+        <v>42</v>
+      </c>
+      <c r="F60" t="s">
+        <v>18</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>1003010204</v>
+      </c>
+      <c r="C61">
+        <v>5001</v>
+      </c>
+      <c r="D61">
+        <v>1003010204</v>
+      </c>
+      <c r="E61" t="s">
+        <v>43</v>
+      </c>
+      <c r="F61" t="s">
+        <v>19</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>1003010205</v>
+      </c>
+      <c r="C62">
+        <v>5001</v>
+      </c>
+      <c r="D62">
+        <v>1003010205</v>
+      </c>
+      <c r="E62" t="s">
         <v>44</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F62" t="s">
         <v>32</v>
       </c>
-      <c r="G59">
+      <c r="G62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="2">
+        <v>10030103</v>
+      </c>
+      <c r="C63" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D63" s="2">
+        <v>10030103</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G63" s="2">
+        <v>1</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>1003010301</v>
+      </c>
+      <c r="C64">
+        <v>5001</v>
+      </c>
+      <c r="D64">
+        <v>1003010301</v>
+      </c>
+      <c r="E64" t="s">
+        <v>40</v>
+      </c>
+      <c r="F64" t="s">
+        <v>16</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>1003010302</v>
+      </c>
+      <c r="C65">
+        <v>5001</v>
+      </c>
+      <c r="D65">
+        <v>1003010302</v>
+      </c>
+      <c r="E65" t="s">
+        <v>41</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>1003010303</v>
+      </c>
+      <c r="C66">
+        <v>5001</v>
+      </c>
+      <c r="D66">
+        <v>1003010303</v>
+      </c>
+      <c r="E66" t="s">
+        <v>42</v>
+      </c>
+      <c r="F66" t="s">
+        <v>18</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>1003010304</v>
+      </c>
+      <c r="C67">
+        <v>5001</v>
+      </c>
+      <c r="D67">
+        <v>1003010304</v>
+      </c>
+      <c r="E67" t="s">
+        <v>43</v>
+      </c>
+      <c r="F67" t="s">
+        <v>19</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>1003010305</v>
+      </c>
+      <c r="C68">
+        <v>5001</v>
+      </c>
+      <c r="D68">
+        <v>1003010305</v>
+      </c>
+      <c r="E68" t="s">
+        <v>44</v>
+      </c>
+      <c r="F68" t="s">
+        <v>32</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="2">
+        <v>10030104</v>
+      </c>
+      <c r="C69" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D69" s="2">
+        <v>10030104</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G69" s="2">
+        <v>1</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>1003010401</v>
+      </c>
+      <c r="C70">
+        <v>5001</v>
+      </c>
+      <c r="D70">
+        <v>1003010401</v>
+      </c>
+      <c r="E70" t="s">
+        <v>40</v>
+      </c>
+      <c r="F70" t="s">
+        <v>16</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>1003010402</v>
+      </c>
+      <c r="C71">
+        <v>5001</v>
+      </c>
+      <c r="D71">
+        <v>1003010402</v>
+      </c>
+      <c r="E71" t="s">
+        <v>41</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <v>1003010403</v>
+      </c>
+      <c r="C72">
+        <v>5001</v>
+      </c>
+      <c r="D72">
+        <v>1003010403</v>
+      </c>
+      <c r="E72" t="s">
+        <v>42</v>
+      </c>
+      <c r="F72" t="s">
+        <v>18</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>1003010404</v>
+      </c>
+      <c r="C73">
+        <v>5001</v>
+      </c>
+      <c r="D73">
+        <v>1003010404</v>
+      </c>
+      <c r="E73" t="s">
+        <v>43</v>
+      </c>
+      <c r="F73" t="s">
+        <v>19</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>1003010405</v>
+      </c>
+      <c r="C74">
+        <v>5001</v>
+      </c>
+      <c r="D74">
+        <v>1003010405</v>
+      </c>
+      <c r="E74" t="s">
+        <v>44</v>
+      </c>
+      <c r="F74" t="s">
+        <v>32</v>
+      </c>
+      <c r="G74">
         <v>1</v>
       </c>
     </row>
@@ -1618,11 +2206,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H52"/>
+  <dimension ref="B1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1632,7 +2220,7 @@
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="92.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
@@ -2067,65 +2655,290 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-    </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="F26" s="3"/>
+      <c r="B26">
+        <v>100201</v>
+      </c>
+      <c r="C26">
+        <v>5000</v>
+      </c>
+      <c r="D26">
+        <v>10020101</v>
+      </c>
+      <c r="E26">
+        <v>5001</v>
+      </c>
+      <c r="F26" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
+      <c r="B27">
+        <v>100201</v>
+      </c>
+      <c r="C27">
+        <v>5000</v>
+      </c>
+      <c r="D27">
+        <v>10020102</v>
+      </c>
+      <c r="E27">
+        <v>5001</v>
+      </c>
+      <c r="F27" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
+      <c r="B28">
+        <v>100201</v>
+      </c>
+      <c r="C28">
+        <v>5000</v>
+      </c>
+      <c r="D28">
+        <v>10020103</v>
+      </c>
+      <c r="E28">
+        <v>5001</v>
+      </c>
+      <c r="F28" t="s">
+        <v>57</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
+      <c r="B29">
+        <v>100201</v>
+      </c>
+      <c r="C29">
+        <v>5000</v>
+      </c>
+      <c r="D29">
+        <v>10020104</v>
+      </c>
+      <c r="E29">
+        <v>5001</v>
+      </c>
+      <c r="F29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>100201</v>
+      </c>
+      <c r="C30">
+        <v>5000</v>
+      </c>
+      <c r="D30">
+        <v>10020105</v>
+      </c>
+      <c r="E30">
+        <v>5001</v>
+      </c>
+      <c r="F30" t="s">
+        <v>59</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>100202</v>
+      </c>
+      <c r="C31">
+        <v>5000</v>
+      </c>
+      <c r="D31">
+        <v>10020201</v>
+      </c>
+      <c r="E31">
+        <v>5001</v>
+      </c>
+      <c r="F31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>100202</v>
+      </c>
+      <c r="C32">
+        <v>5000</v>
+      </c>
+      <c r="D32">
+        <v>10020202</v>
+      </c>
+      <c r="E32">
+        <v>5001</v>
+      </c>
+      <c r="F32" t="s">
+        <v>66</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>100202</v>
+      </c>
+      <c r="C33">
+        <v>5000</v>
+      </c>
+      <c r="D33">
+        <v>10020203</v>
+      </c>
+      <c r="E33">
+        <v>5001</v>
+      </c>
+      <c r="F33" t="s">
+        <v>67</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>100202</v>
+      </c>
+      <c r="C34">
+        <v>5000</v>
+      </c>
+      <c r="D34">
+        <v>10020204</v>
+      </c>
+      <c r="E34">
+        <v>5001</v>
+      </c>
+      <c r="F34" t="s">
+        <v>68</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>100202</v>
+      </c>
+      <c r="C35">
+        <v>5000</v>
+      </c>
+      <c r="D35">
+        <v>10020205</v>
+      </c>
+      <c r="E35">
+        <v>5001</v>
+      </c>
+      <c r="F35" t="s">
+        <v>69</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="2">
+        <v>100203</v>
+      </c>
+      <c r="C36" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D36" s="2">
+        <v>10020301</v>
+      </c>
+      <c r="E36" s="2">
+        <v>5001</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G36" s="2">
+        <v>1</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>100203</v>
+      </c>
+      <c r="C37">
+        <v>5000</v>
+      </c>
+      <c r="D37">
+        <v>10020302</v>
+      </c>
+      <c r="E37">
+        <v>5001</v>
+      </c>
+      <c r="F37" t="s">
+        <v>74</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38">
-        <v>100201</v>
+        <v>100203</v>
       </c>
       <c r="C38">
         <v>5000</v>
       </c>
       <c r="D38">
-        <v>10020101</v>
+        <v>10020303</v>
       </c>
       <c r="E38">
         <v>5001</v>
       </c>
       <c r="F38" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="G38">
         <v>1</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39">
-        <v>100201</v>
+        <v>100203</v>
       </c>
       <c r="C39">
         <v>5000</v>
       </c>
       <c r="D39">
-        <v>10020102</v>
+        <v>10020304</v>
       </c>
       <c r="E39">
         <v>5001</v>
       </c>
       <c r="F39" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="G39">
         <v>1</v>
@@ -2133,269 +2946,438 @@
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40">
-        <v>100201</v>
+        <v>100203</v>
       </c>
       <c r="C40">
         <v>5000</v>
       </c>
       <c r="D40">
-        <v>10020103</v>
+        <v>10020305</v>
       </c>
       <c r="E40">
         <v>5001</v>
       </c>
       <c r="F40" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="G40">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41">
-        <v>100201</v>
-      </c>
-      <c r="C41">
-        <v>5000</v>
-      </c>
-      <c r="D41">
-        <v>10020104</v>
-      </c>
-      <c r="E41">
-        <v>5001</v>
-      </c>
-      <c r="F41" t="s">
-        <v>58</v>
-      </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42">
-        <v>100201</v>
-      </c>
-      <c r="C42">
-        <v>5000</v>
-      </c>
-      <c r="D42">
-        <v>10020105</v>
-      </c>
-      <c r="E42">
-        <v>5001</v>
-      </c>
-      <c r="F42" t="s">
-        <v>59</v>
-      </c>
-      <c r="G42">
-        <v>1</v>
+    <row r="42" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="2">
+        <v>10030101</v>
+      </c>
+      <c r="C42" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D42" s="2">
+        <v>1003010101</v>
+      </c>
+      <c r="E42" s="2">
+        <v>5001</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G42" s="2">
+        <v>1</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43">
-        <v>100202</v>
+      <c r="B43" s="3">
+        <v>10030101</v>
       </c>
       <c r="C43">
         <v>5000</v>
       </c>
       <c r="D43">
-        <v>10020201</v>
+        <v>1003010102</v>
       </c>
       <c r="E43">
         <v>5001</v>
       </c>
-      <c r="F43" t="s">
-        <v>65</v>
+      <c r="F43" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="G43">
         <v>1</v>
       </c>
-      <c r="H43" s="2" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44">
-        <v>100202</v>
+      <c r="B44" s="3">
+        <v>10030101</v>
       </c>
       <c r="C44">
         <v>5000</v>
       </c>
       <c r="D44">
-        <v>10020202</v>
+        <v>1003010103</v>
       </c>
       <c r="E44">
         <v>5001</v>
       </c>
       <c r="F44" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="G44">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45">
-        <v>100202</v>
+      <c r="B45" s="3">
+        <v>10030101</v>
       </c>
       <c r="C45">
         <v>5000</v>
       </c>
       <c r="D45">
-        <v>10020203</v>
+        <v>1003010104</v>
       </c>
       <c r="E45">
         <v>5001</v>
       </c>
       <c r="F45" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="G45">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46">
-        <v>100202</v>
+      <c r="B46" s="3">
+        <v>10030101</v>
       </c>
       <c r="C46">
         <v>5000</v>
       </c>
       <c r="D46">
-        <v>10020204</v>
+        <v>1003010105</v>
       </c>
       <c r="E46">
         <v>5001</v>
       </c>
       <c r="F46" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="G46">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47">
-        <v>100202</v>
-      </c>
-      <c r="C47">
-        <v>5000</v>
-      </c>
-      <c r="D47">
-        <v>10020205</v>
-      </c>
-      <c r="E47">
-        <v>5001</v>
-      </c>
-      <c r="F47" t="s">
-        <v>69</v>
-      </c>
-      <c r="G47">
-        <v>1</v>
+    <row r="47" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="2">
+        <v>10030102</v>
+      </c>
+      <c r="C47" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D47" s="2">
+        <v>1003010201</v>
+      </c>
+      <c r="E47" s="2">
+        <v>5001</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G47" s="2">
+        <v>1</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="2">
-        <v>100203</v>
-      </c>
-      <c r="C48" s="2">
-        <v>5000</v>
-      </c>
-      <c r="D48" s="2">
-        <v>10020301</v>
-      </c>
-      <c r="E48" s="2">
-        <v>5001</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G48" s="2">
-        <v>1</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49">
-        <v>100203</v>
+      <c r="B48" s="3">
+        <v>10030102</v>
+      </c>
+      <c r="C48">
+        <v>5000</v>
+      </c>
+      <c r="D48">
+        <v>1003010202</v>
+      </c>
+      <c r="E48">
+        <v>5001</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="3">
+        <v>10030102</v>
       </c>
       <c r="C49">
         <v>5000</v>
       </c>
       <c r="D49">
-        <v>10020302</v>
+        <v>1003010203</v>
       </c>
       <c r="E49">
         <v>5001</v>
       </c>
       <c r="F49" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="G49">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50">
-        <v>100203</v>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="3">
+        <v>10030102</v>
       </c>
       <c r="C50">
         <v>5000</v>
       </c>
       <c r="D50">
-        <v>10020303</v>
+        <v>1003010204</v>
       </c>
       <c r="E50">
         <v>5001</v>
       </c>
       <c r="F50" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G50">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51">
-        <v>100203</v>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="3">
+        <v>10030102</v>
       </c>
       <c r="C51">
         <v>5000</v>
       </c>
       <c r="D51">
-        <v>10020304</v>
+        <v>1003010205</v>
       </c>
       <c r="E51">
         <v>5001</v>
       </c>
       <c r="F51" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="G51">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52">
-        <v>100203</v>
-      </c>
-      <c r="C52">
-        <v>5000</v>
-      </c>
-      <c r="D52">
-        <v>10020305</v>
-      </c>
-      <c r="E52">
-        <v>5001</v>
-      </c>
-      <c r="F52" t="s">
-        <v>77</v>
-      </c>
-      <c r="G52">
-        <v>1</v>
-      </c>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="2">
+        <v>10030103</v>
+      </c>
+      <c r="C52" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D52" s="2">
+        <v>1003010301</v>
+      </c>
+      <c r="E52" s="2">
+        <v>5001</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G52" s="2">
+        <v>1</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="3">
+        <v>10030103</v>
+      </c>
+      <c r="C53">
+        <v>5000</v>
+      </c>
+      <c r="D53">
+        <v>1003010302</v>
+      </c>
+      <c r="E53">
+        <v>5001</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="3">
+        <v>10030103</v>
+      </c>
+      <c r="C54">
+        <v>5000</v>
+      </c>
+      <c r="D54">
+        <v>1003010303</v>
+      </c>
+      <c r="E54">
+        <v>5001</v>
+      </c>
+      <c r="F54" t="s">
+        <v>83</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="3">
+        <v>10030103</v>
+      </c>
+      <c r="C55">
+        <v>5000</v>
+      </c>
+      <c r="D55">
+        <v>1003010304</v>
+      </c>
+      <c r="E55">
+        <v>5001</v>
+      </c>
+      <c r="F55" t="s">
+        <v>84</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="3">
+        <v>10030103</v>
+      </c>
+      <c r="C56">
+        <v>5000</v>
+      </c>
+      <c r="D56">
+        <v>1003010305</v>
+      </c>
+      <c r="E56">
+        <v>5001</v>
+      </c>
+      <c r="F56" t="s">
+        <v>85</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="2">
+        <v>10030104</v>
+      </c>
+      <c r="C57" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D57" s="2">
+        <v>1003010401</v>
+      </c>
+      <c r="E57" s="2">
+        <v>5001</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G57" s="2">
+        <v>1</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="2">
+        <v>10030104</v>
+      </c>
+      <c r="C58">
+        <v>5000</v>
+      </c>
+      <c r="D58">
+        <v>1003010402</v>
+      </c>
+      <c r="E58">
+        <v>5001</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="2">
+        <v>10030104</v>
+      </c>
+      <c r="C59">
+        <v>5000</v>
+      </c>
+      <c r="D59">
+        <v>1003010403</v>
+      </c>
+      <c r="E59">
+        <v>5001</v>
+      </c>
+      <c r="F59" t="s">
+        <v>101</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="2">
+        <v>10030104</v>
+      </c>
+      <c r="C60">
+        <v>5000</v>
+      </c>
+      <c r="D60">
+        <v>1003010404</v>
+      </c>
+      <c r="E60">
+        <v>5001</v>
+      </c>
+      <c r="F60" t="s">
+        <v>102</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="2">
+        <v>10030104</v>
+      </c>
+      <c r="C61">
+        <v>5000</v>
+      </c>
+      <c r="D61">
+        <v>1003010405</v>
+      </c>
+      <c r="E61">
+        <v>5001</v>
+      </c>
+      <c r="F61" t="s">
+        <v>103</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2405,11 +3387,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I62"/>
+  <dimension ref="B1:I75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I28" sqref="I28"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F70" sqref="F70:F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3036,80 +4018,383 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-    </row>
+    <row r="28" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="2">
-        <v>1</v>
-      </c>
-      <c r="C44" s="2">
+    <row r="30" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2">
         <v>10</v>
       </c>
-      <c r="D44" s="2">
-        <v>1</v>
-      </c>
-      <c r="E44" s="2">
-        <v>5000</v>
-      </c>
-      <c r="F44" s="2">
+      <c r="D30" s="2">
+        <v>1</v>
+      </c>
+      <c r="E30" s="2">
+        <v>5000</v>
+      </c>
+      <c r="F30" s="2">
         <v>1002</v>
       </c>
-      <c r="G44" s="2">
-        <v>0</v>
-      </c>
-      <c r="H44" s="2">
-        <v>1</v>
-      </c>
-      <c r="I44" s="2" t="s">
+      <c r="G30" s="2">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2">
+        <v>1</v>
+      </c>
+      <c r="I30" s="2" t="s">
         <v>63</v>
       </c>
     </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="2">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2">
+        <v>10</v>
+      </c>
+      <c r="D31" s="2">
+        <v>1</v>
+      </c>
+      <c r="E31" s="2">
+        <v>5000</v>
+      </c>
+      <c r="F31" s="2">
+        <v>100201</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2">
+        <v>1</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>5001</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>5001</v>
+      </c>
+      <c r="F32">
+        <v>10020101</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>5001</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>5001</v>
+      </c>
+      <c r="F33">
+        <v>10020102</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>5001</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>5001</v>
+      </c>
+      <c r="F34">
+        <v>10020103</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>5001</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>5001</v>
+      </c>
+      <c r="F35">
+        <v>10020104</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>5001</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>5001</v>
+      </c>
+      <c r="F36">
+        <v>10020105</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2">
+        <v>10</v>
+      </c>
+      <c r="D37" s="2">
+        <v>1</v>
+      </c>
+      <c r="E37" s="2">
+        <v>5000</v>
+      </c>
+      <c r="F37" s="2">
+        <v>100202</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0</v>
+      </c>
+      <c r="H37" s="2">
+        <v>1</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>5001</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>5001</v>
+      </c>
+      <c r="F38">
+        <v>10020201</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>5001</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>5001</v>
+      </c>
+      <c r="F39">
+        <v>10020202</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>5001</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>5001</v>
+      </c>
+      <c r="F40">
+        <v>10020203</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>5001</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>5001</v>
+      </c>
+      <c r="F41">
+        <v>10020204</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>5001</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>5001</v>
+      </c>
+      <c r="F42">
+        <v>10020205</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="2">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2">
+        <v>10</v>
+      </c>
+      <c r="D43" s="2">
+        <v>1</v>
+      </c>
+      <c r="E43" s="2">
+        <v>5000</v>
+      </c>
+      <c r="F43" s="2">
+        <v>100203</v>
+      </c>
+      <c r="G43" s="2">
+        <v>0</v>
+      </c>
+      <c r="H43" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>5001</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>5001</v>
+      </c>
+      <c r="F44">
+        <v>10020301</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+    </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="2">
-        <v>1</v>
-      </c>
-      <c r="C45" s="2">
-        <v>10</v>
-      </c>
-      <c r="D45" s="2">
-        <v>1</v>
-      </c>
-      <c r="E45" s="2">
-        <v>5000</v>
-      </c>
-      <c r="F45" s="2">
-        <v>100201</v>
-      </c>
-      <c r="G45" s="2">
-        <v>0</v>
-      </c>
-      <c r="H45" s="2">
-        <v>1</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>48</v>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>5001</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>5001</v>
+      </c>
+      <c r="F45">
+        <v>10020302</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
@@ -3126,7 +4411,7 @@
         <v>5001</v>
       </c>
       <c r="F46">
-        <v>10020101</v>
+        <v>10020303</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -3149,7 +4434,7 @@
         <v>5001</v>
       </c>
       <c r="F47">
-        <v>10020102</v>
+        <v>10020304</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -3172,7 +4457,7 @@
         <v>5001</v>
       </c>
       <c r="F48">
-        <v>10020103</v>
+        <v>10020305</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -3181,50 +4466,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="C49">
-        <v>5001</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="E49">
-        <v>5001</v>
-      </c>
-      <c r="F49">
-        <v>10020104</v>
-      </c>
-      <c r="G49">
-        <v>0</v>
-      </c>
-      <c r="H49">
-        <v>1</v>
-      </c>
-    </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50">
-        <v>1</v>
-      </c>
-      <c r="C50">
-        <v>5001</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-      <c r="E50">
-        <v>5001</v>
-      </c>
-      <c r="F50">
-        <v>10020105</v>
-      </c>
-      <c r="G50">
-        <v>0</v>
-      </c>
-      <c r="H50">
-        <v>1</v>
+      <c r="B50" s="2">
+        <v>1</v>
+      </c>
+      <c r="C50" s="2">
+        <v>10</v>
+      </c>
+      <c r="D50" s="2">
+        <v>1</v>
+      </c>
+      <c r="E50" s="2">
+        <v>5000</v>
+      </c>
+      <c r="F50" s="2">
+        <v>1003</v>
+      </c>
+      <c r="G50" s="2">
+        <v>0</v>
+      </c>
+      <c r="H50" s="2">
+        <v>1</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
@@ -3240,8 +4505,8 @@
       <c r="E51" s="2">
         <v>5000</v>
       </c>
-      <c r="F51" s="2">
-        <v>100202</v>
+      <c r="F51">
+        <v>100301</v>
       </c>
       <c r="G51" s="2">
         <v>0</v>
@@ -3250,30 +4515,33 @@
         <v>1</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B52">
-        <v>1</v>
-      </c>
-      <c r="C52">
-        <v>5001</v>
-      </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-      <c r="E52">
-        <v>5001</v>
-      </c>
-      <c r="F52">
-        <v>10020201</v>
-      </c>
-      <c r="G52">
-        <v>0</v>
-      </c>
-      <c r="H52">
-        <v>1</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="2">
+        <v>1</v>
+      </c>
+      <c r="C52" s="2">
+        <v>10</v>
+      </c>
+      <c r="D52" s="2">
+        <v>1</v>
+      </c>
+      <c r="E52" s="2">
+        <v>5000</v>
+      </c>
+      <c r="F52" s="2">
+        <v>10030101</v>
+      </c>
+      <c r="G52" s="2">
+        <v>0</v>
+      </c>
+      <c r="H52" s="2">
+        <v>1</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
@@ -3290,7 +4558,7 @@
         <v>5001</v>
       </c>
       <c r="F53">
-        <v>10020202</v>
+        <v>1003010101</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -3313,7 +4581,7 @@
         <v>5001</v>
       </c>
       <c r="F54">
-        <v>10020203</v>
+        <v>1003010102</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -3336,7 +4604,7 @@
         <v>5001</v>
       </c>
       <c r="F55">
-        <v>10020204</v>
+        <v>1003010103</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -3359,7 +4627,7 @@
         <v>5001</v>
       </c>
       <c r="F56">
-        <v>10020205</v>
+        <v>1003010104</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -3369,49 +4637,52 @@
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B57" s="2">
-        <v>1</v>
-      </c>
-      <c r="C57" s="2">
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>5001</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>5001</v>
+      </c>
+      <c r="F57">
+        <v>1003010105</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="2">
+        <v>1</v>
+      </c>
+      <c r="C58" s="2">
         <v>10</v>
       </c>
-      <c r="D57" s="2">
-        <v>1</v>
-      </c>
-      <c r="E57" s="2">
-        <v>5000</v>
-      </c>
-      <c r="F57" s="2">
-        <v>100203</v>
-      </c>
-      <c r="G57" s="2">
-        <v>0</v>
-      </c>
-      <c r="H57" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B58">
-        <v>1</v>
-      </c>
-      <c r="C58">
-        <v>5001</v>
-      </c>
-      <c r="D58">
-        <v>1</v>
-      </c>
-      <c r="E58">
-        <v>5001</v>
-      </c>
-      <c r="F58">
-        <v>10020301</v>
-      </c>
-      <c r="G58">
-        <v>0</v>
-      </c>
-      <c r="H58">
-        <v>1</v>
+      <c r="D58" s="2">
+        <v>1</v>
+      </c>
+      <c r="E58" s="2">
+        <v>5000</v>
+      </c>
+      <c r="F58" s="2">
+        <v>10030102</v>
+      </c>
+      <c r="G58" s="2">
+        <v>0</v>
+      </c>
+      <c r="H58" s="2">
+        <v>1</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
@@ -3428,7 +4699,7 @@
         <v>5001</v>
       </c>
       <c r="F59">
-        <v>10020302</v>
+        <v>1003010201</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -3451,7 +4722,7 @@
         <v>5001</v>
       </c>
       <c r="F60">
-        <v>10020303</v>
+        <v>1003010202</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -3474,7 +4745,7 @@
         <v>5001</v>
       </c>
       <c r="F61">
-        <v>10020304</v>
+        <v>1003010203</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -3497,12 +4768,317 @@
         <v>5001</v>
       </c>
       <c r="F62">
-        <v>10020305</v>
+        <v>1003010204</v>
       </c>
       <c r="G62">
         <v>0</v>
       </c>
       <c r="H62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>5001</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>5001</v>
+      </c>
+      <c r="F63">
+        <v>1003010205</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="2">
+        <v>1</v>
+      </c>
+      <c r="C64" s="2">
+        <v>10</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1</v>
+      </c>
+      <c r="E64" s="2">
+        <v>5000</v>
+      </c>
+      <c r="F64" s="2">
+        <v>10030103</v>
+      </c>
+      <c r="G64" s="2">
+        <v>0</v>
+      </c>
+      <c r="H64" s="2">
+        <v>1</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65">
+        <v>5001</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>5001</v>
+      </c>
+      <c r="F65">
+        <v>1003010301</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>5001</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>5001</v>
+      </c>
+      <c r="F66">
+        <v>1003010302</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>5001</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>5001</v>
+      </c>
+      <c r="F67">
+        <v>1003010303</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <v>5001</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>5001</v>
+      </c>
+      <c r="F68">
+        <v>1003010304</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69">
+        <v>5001</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>5001</v>
+      </c>
+      <c r="F69">
+        <v>1003010305</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B70" s="2">
+        <v>1</v>
+      </c>
+      <c r="C70" s="2">
+        <v>10</v>
+      </c>
+      <c r="D70" s="2">
+        <v>1</v>
+      </c>
+      <c r="E70" s="2">
+        <v>5000</v>
+      </c>
+      <c r="F70" s="2">
+        <v>10030104</v>
+      </c>
+      <c r="G70" s="2">
+        <v>0</v>
+      </c>
+      <c r="H70" s="2">
+        <v>1</v>
+      </c>
+      <c r="I70" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <v>5001</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>5001</v>
+      </c>
+      <c r="F71">
+        <v>1003010401</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72">
+        <v>5001</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>5001</v>
+      </c>
+      <c r="F72">
+        <v>1003010402</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73">
+        <v>5001</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>5001</v>
+      </c>
+      <c r="F73">
+        <v>1003010403</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74">
+        <v>5001</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <v>5001</v>
+      </c>
+      <c r="F74">
+        <v>1003010404</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75">
+        <v>5001</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <v>5001</v>
+      </c>
+      <c r="F75">
+        <v>1003010405</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Hasta Series Ok - Asignadas para empresa diferente
</commit_message>
<xml_diff>
--- a/Documentacion APPs/Documentacion SA - MENUS.xlsx
+++ b/Documentacion APPs/Documentacion SA - MENUS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="112">
   <si>
     <t>nParCodigo</t>
   </si>
@@ -333,13 +333,25 @@
     <t>PUNTOS DE EMISION</t>
   </si>
   <si>
-    <t>xajax_Configurar_Parametro(1009);</t>
-  </si>
-  <si>
     <t>Punto de Emisión</t>
   </si>
   <si>
     <t>PUNTOS DE EMISON</t>
+  </si>
+  <si>
+    <t>xajax_Listar_Series_Empresa(0,20,1,1);</t>
+  </si>
+  <si>
+    <t>xajax_Editar_Serie_Empresa(xajax.getFormValues(FrmPrincipal));</t>
+  </si>
+  <si>
+    <t>xajax_Eliminar_Serie_Empresa(xajax.getFormValues(FrmPrincipal));</t>
+  </si>
+  <si>
+    <t>xajax_Rpt_Serie_Empresa_Pdf(xajax.getFormValues(FrmPrincipal));</t>
+  </si>
+  <si>
+    <t>xajax_Nuevo_Serie_Empresa();</t>
   </si>
 </sst>
 </file>
@@ -697,8 +709,8 @@
   <dimension ref="B1:H74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B63" sqref="B63:H68"/>
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,7 +718,7 @@
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.28515625" style="2" bestFit="1" customWidth="1"/>
@@ -1720,7 +1732,7 @@
         <v>90</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G51" s="2">
         <v>1</v>
@@ -1963,7 +1975,7 @@
         <v>10030103</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>92</v>
@@ -2210,7 +2222,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
+      <selection pane="bottomLeft" activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2984,7 +2996,7 @@
         <v>1</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
@@ -3184,7 +3196,7 @@
         <v>5001</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="G52" s="2">
         <v>1</v>
@@ -3206,8 +3218,8 @@
       <c r="E53">
         <v>5001</v>
       </c>
-      <c r="F53" s="3" t="s">
-        <v>105</v>
+      <c r="F53" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="G53">
         <v>1</v>
@@ -3227,7 +3239,7 @@
         <v>5001</v>
       </c>
       <c r="F54" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="G54">
         <v>1</v>
@@ -3247,7 +3259,7 @@
         <v>5001</v>
       </c>
       <c r="F55" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="G55">
         <v>1</v>
@@ -3267,7 +3279,7 @@
         <v>5001</v>
       </c>
       <c r="F56" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="G56">
         <v>1</v>
@@ -3309,8 +3321,8 @@
       <c r="E58">
         <v>5001</v>
       </c>
-      <c r="F58" s="3" t="s">
-        <v>99</v>
+      <c r="F58" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="G58">
         <v>1</v>

</xml_diff>

<commit_message>
Hasta el Listar Asignacion de comprobante a la Serio y Numeracion
</commit_message>
<xml_diff>
--- a/Documentacion APPs/Documentacion SA - MENUS.xlsx
+++ b/Documentacion APPs/Documentacion SA - MENUS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Parametro" sheetId="1" r:id="rId1"/>
@@ -315,21 +315,6 @@
     <t>Asignar Series</t>
   </si>
   <si>
-    <t>xajax_Listar_AsignarSeries(0,20,1,1);</t>
-  </si>
-  <si>
-    <t>xajax_Nuevo_AsignarSerie();</t>
-  </si>
-  <si>
-    <t>xajax_Editar_AsignarSerie(xajax.getFormValues(FrmPrincipal));</t>
-  </si>
-  <si>
-    <t>xajax_Eliminar_AsignarSerie(xajax.getFormValues(FrmPrincipal));</t>
-  </si>
-  <si>
-    <t>xajax_Rpt_AsignarSerie_Pdf(xajax.getFormValues(FrmPrincipal));</t>
-  </si>
-  <si>
     <t>PUNTOS DE EMISION</t>
   </si>
   <si>
@@ -352,6 +337,21 @@
   </si>
   <si>
     <t>xajax_Nuevo_Serie_Empresa();</t>
+  </si>
+  <si>
+    <t>xajax_Nuevo_Serie_Numeracion();</t>
+  </si>
+  <si>
+    <t>xajax_Listar_Series_Numeracion(0,20,1,1);</t>
+  </si>
+  <si>
+    <t>xajax_Editar_Serie_Numeracion(xajax.getFormValues(FrmPrincipal));</t>
+  </si>
+  <si>
+    <t>xajax_Eliminar_Serie_Numeracion(xajax.getFormValues(FrmPrincipal));</t>
+  </si>
+  <si>
+    <t>xajax_Rpt_Serie_Numeracion_Pdf(xajax.getFormValues(FrmPrincipal));</t>
   </si>
 </sst>
 </file>
@@ -708,9 +708,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,13 +1732,13 @@
         <v>90</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G51" s="2">
         <v>1</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
@@ -1975,7 +1975,7 @@
         <v>10030103</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>92</v>
@@ -2098,7 +2098,7 @@
         <v>10030104</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>98</v>
@@ -2220,9 +2220,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F52" sqref="F52"/>
+      <selection pane="bottomLeft" activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2996,7 +2996,7 @@
         <v>1</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
@@ -3196,7 +3196,7 @@
         <v>5001</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G52" s="2">
         <v>1</v>
@@ -3219,7 +3219,7 @@
         <v>5001</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G53">
         <v>1</v>
@@ -3239,7 +3239,7 @@
         <v>5001</v>
       </c>
       <c r="F54" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G54">
         <v>1</v>
@@ -3259,7 +3259,7 @@
         <v>5001</v>
       </c>
       <c r="F55" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G55">
         <v>1</v>
@@ -3279,7 +3279,7 @@
         <v>5001</v>
       </c>
       <c r="F56" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G56">
         <v>1</v>
@@ -3299,7 +3299,7 @@
         <v>5001</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="G57" s="2">
         <v>1</v>
@@ -3322,7 +3322,7 @@
         <v>5001</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G58">
         <v>1</v>
@@ -3342,7 +3342,7 @@
         <v>5001</v>
       </c>
       <c r="F59" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="G59">
         <v>1</v>
@@ -3362,7 +3362,7 @@
         <v>5001</v>
       </c>
       <c r="F60" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="G60">
         <v>1</v>
@@ -3382,7 +3382,7 @@
         <v>5001</v>
       </c>
       <c r="F61" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="G61">
         <v>1</v>
@@ -4553,7 +4553,7 @@
         <v>1</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Sin la Capa Models
</commit_message>
<xml_diff>
--- a/Documentacion APPs/Documentacion SA - MENUS.xlsx
+++ b/Documentacion APPs/Documentacion SA - MENUS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Parametro" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="116">
   <si>
     <t>nParCodigo</t>
   </si>
@@ -252,9 +252,6 @@
     <t>xajax_Rpt_Cosecha_Pdf(xajax.getFormValues(FrmPrincipal));</t>
   </si>
   <si>
-    <t>xajax_Configurar_Parametro(2007);</t>
-  </si>
-  <si>
     <t>PRODUCTOS</t>
   </si>
   <si>
@@ -352,6 +349,21 @@
   </si>
   <si>
     <t>xajax_Rpt_Serie_Numeracion_Pdf(xajax.getFormValues(FrmPrincipal));</t>
+  </si>
+  <si>
+    <t>xajax_Listar_Productos(0,20,1,1);</t>
+  </si>
+  <si>
+    <t>xajax_Nuevo_Producto();</t>
+  </si>
+  <si>
+    <t>xajax_Editar_Producto(xajax.getFormValues(FrmPrincipal));</t>
+  </si>
+  <si>
+    <t>xajax_Eliminar_Producto(xajax.getFormValues(FrmPrincipal));</t>
+  </si>
+  <si>
+    <t>xajax_Rpt_Producto_Pdf(xajax.getFormValues(FrmPrincipal));</t>
   </si>
 </sst>
 </file>
@@ -708,9 +720,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E69" sqref="E69"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,16 +1182,16 @@
         <v>100104</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="F22" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="G22" s="2">
-        <v>1</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -1688,13 +1700,13 @@
         <v>7</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G49" s="2">
         <v>1</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
@@ -1709,13 +1721,13 @@
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G50" s="2">
         <v>1</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
@@ -1729,16 +1741,16 @@
         <v>10030101</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G51" s="2">
         <v>1</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
@@ -1852,16 +1864,16 @@
         <v>10030102</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F57" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G57" s="2">
+        <v>1</v>
+      </c>
+      <c r="H57" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="G57" s="2">
-        <v>1</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
@@ -1975,16 +1987,16 @@
         <v>10030103</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G63" s="2">
         <v>1</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
@@ -2098,16 +2110,16 @@
         <v>10030104</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G69" s="2">
         <v>1</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
@@ -2220,9 +2232,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H65"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2558,7 +2570,7 @@
         <v>5001</v>
       </c>
       <c r="F19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -2578,13 +2590,13 @@
         <v>5001</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="G20" s="2">
         <v>1</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -2600,8 +2612,8 @@
       <c r="E21">
         <v>5001</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>78</v>
+      <c r="F21" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -2621,7 +2633,7 @@
         <v>5001</v>
       </c>
       <c r="F22" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -2641,7 +2653,7 @@
         <v>5001</v>
       </c>
       <c r="F23" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -2661,7 +2673,7 @@
         <v>5001</v>
       </c>
       <c r="F24" t="s">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -2990,13 +3002,13 @@
         <v>5001</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G42" s="2">
         <v>1</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
@@ -3013,7 +3025,7 @@
         <v>5001</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -3033,7 +3045,7 @@
         <v>5001</v>
       </c>
       <c r="F44" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G44">
         <v>1</v>
@@ -3053,7 +3065,7 @@
         <v>5001</v>
       </c>
       <c r="F45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G45">
         <v>1</v>
@@ -3073,7 +3085,7 @@
         <v>5001</v>
       </c>
       <c r="F46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G46">
         <v>1</v>
@@ -3093,13 +3105,13 @@
         <v>5001</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G47" s="2">
         <v>1</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
@@ -3116,7 +3128,7 @@
         <v>5001</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G48">
         <v>1</v>
@@ -3136,7 +3148,7 @@
         <v>5001</v>
       </c>
       <c r="F49" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G49">
         <v>1</v>
@@ -3156,7 +3168,7 @@
         <v>5001</v>
       </c>
       <c r="F50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G50">
         <v>1</v>
@@ -3176,7 +3188,7 @@
         <v>5001</v>
       </c>
       <c r="F51" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G51">
         <v>1</v>
@@ -3196,13 +3208,13 @@
         <v>5001</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G52" s="2">
         <v>1</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
@@ -3219,7 +3231,7 @@
         <v>5001</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G53">
         <v>1</v>
@@ -3239,7 +3251,7 @@
         <v>5001</v>
       </c>
       <c r="F54" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G54">
         <v>1</v>
@@ -3259,7 +3271,7 @@
         <v>5001</v>
       </c>
       <c r="F55" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G55">
         <v>1</v>
@@ -3279,7 +3291,7 @@
         <v>5001</v>
       </c>
       <c r="F56" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G56">
         <v>1</v>
@@ -3299,13 +3311,13 @@
         <v>5001</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G57" s="2">
         <v>1</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
@@ -3322,7 +3334,7 @@
         <v>5001</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G58">
         <v>1</v>
@@ -3342,7 +3354,7 @@
         <v>5001</v>
       </c>
       <c r="F59" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G59">
         <v>1</v>
@@ -3362,7 +3374,7 @@
         <v>5001</v>
       </c>
       <c r="F60" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G60">
         <v>1</v>
@@ -3382,7 +3394,7 @@
         <v>5001</v>
       </c>
       <c r="F61" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G61">
         <v>1</v>
@@ -3912,7 +3924,7 @@
         <v>1</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4501,7 +4513,7 @@
         <v>1</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
@@ -4527,7 +4539,7 @@
         <v>1</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4553,7 +4565,7 @@
         <v>1</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
@@ -4694,7 +4706,7 @@
         <v>1</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
@@ -4835,7 +4847,7 @@
         <v>1</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
@@ -4976,7 +4988,7 @@
         <v>1</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Hasta Cargar Formulario Comprobante de Entrada
</commit_message>
<xml_diff>
--- a/Documentacion APPs/Documentacion SA - MENUS.xlsx
+++ b/Documentacion APPs/Documentacion SA - MENUS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="121">
   <si>
     <t>nParCodigo</t>
   </si>
@@ -364,13 +364,28 @@
   </si>
   <si>
     <t>xajax_Rpt_Producto_Pdf(xajax.getFormValues(FrmPrincipal));</t>
+  </si>
+  <si>
+    <t>MAESTRO ACOPIO</t>
+  </si>
+  <si>
+    <t>Acopio</t>
+  </si>
+  <si>
+    <t>Comprobante Entrada</t>
+  </si>
+  <si>
+    <t>xajax_Nuevo_Comprob_Entrada();</t>
+  </si>
+  <si>
+    <t>xajax_Listar_Comprob_Entradas(0,20,1,1);</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,6 +397,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -407,13 +437,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -718,11 +750,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H74"/>
+  <dimension ref="B1:H82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,7 +762,7 @@
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.28515625" style="2" bestFit="1" customWidth="1"/>
@@ -2221,6 +2253,155 @@
       <c r="G74">
         <v>1</v>
       </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="2">
+        <v>1004</v>
+      </c>
+      <c r="C76" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D76" s="2">
+        <v>1004</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G76" s="2">
+        <v>1</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="2">
+        <v>100401</v>
+      </c>
+      <c r="C77" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D77" s="2">
+        <v>100401</v>
+      </c>
+      <c r="E77" t="s">
+        <v>120</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G77" s="2">
+        <v>1</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>10040101</v>
+      </c>
+      <c r="C78">
+        <v>5001</v>
+      </c>
+      <c r="D78">
+        <v>10040101</v>
+      </c>
+      <c r="E78" t="s">
+        <v>40</v>
+      </c>
+      <c r="F78" t="s">
+        <v>16</v>
+      </c>
+      <c r="G78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>10040102</v>
+      </c>
+      <c r="C79">
+        <v>5001</v>
+      </c>
+      <c r="D79">
+        <v>10040102</v>
+      </c>
+      <c r="E79" t="s">
+        <v>41</v>
+      </c>
+      <c r="F79" t="s">
+        <v>17</v>
+      </c>
+      <c r="G79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="4">
+        <v>10040103</v>
+      </c>
+      <c r="C80" s="4">
+        <v>5001</v>
+      </c>
+      <c r="D80" s="4">
+        <v>10040103</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G80" s="4">
+        <v>1</v>
+      </c>
+      <c r="H80" s="5"/>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="4">
+        <v>10040104</v>
+      </c>
+      <c r="C81" s="4">
+        <v>5001</v>
+      </c>
+      <c r="D81" s="4">
+        <v>10040104</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G81" s="4">
+        <v>1</v>
+      </c>
+      <c r="H81" s="5"/>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B82" s="4">
+        <v>10040105</v>
+      </c>
+      <c r="C82" s="4">
+        <v>5001</v>
+      </c>
+      <c r="D82" s="4">
+        <v>10040105</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G82" s="4">
+        <v>1</v>
+      </c>
+      <c r="H82" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2230,11 +2411,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H65"/>
+  <dimension ref="B1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F63" sqref="F63:F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3321,7 +3502,7 @@
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B58" s="2">
+      <c r="B58" s="3">
         <v>10030104</v>
       </c>
       <c r="C58">
@@ -3333,7 +3514,7 @@
       <c r="E58">
         <v>5001</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="F58" s="3" t="s">
         <v>107</v>
       </c>
       <c r="G58">
@@ -3341,7 +3522,7 @@
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B59" s="2">
+      <c r="B59" s="3">
         <v>10030104</v>
       </c>
       <c r="C59">
@@ -3361,7 +3542,7 @@
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B60" s="2">
+      <c r="B60" s="3">
         <v>10030104</v>
       </c>
       <c r="C60">
@@ -3381,7 +3562,7 @@
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="2">
+      <c r="B61" s="3">
         <v>10030104</v>
       </c>
       <c r="C61">
@@ -3400,8 +3581,108 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D65" s="2"/>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="2">
+        <v>100401</v>
+      </c>
+      <c r="C63">
+        <v>5000</v>
+      </c>
+      <c r="D63">
+        <v>10040101</v>
+      </c>
+      <c r="E63">
+        <v>5001</v>
+      </c>
+      <c r="F63" t="s">
+        <v>119</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="3">
+        <v>100401</v>
+      </c>
+      <c r="C64">
+        <v>5000</v>
+      </c>
+      <c r="D64">
+        <v>10040102</v>
+      </c>
+      <c r="E64">
+        <v>5001</v>
+      </c>
+      <c r="F64" t="s">
+        <v>120</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="4">
+        <v>100401</v>
+      </c>
+      <c r="C65" s="4">
+        <v>5000</v>
+      </c>
+      <c r="D65" s="4">
+        <v>10040103</v>
+      </c>
+      <c r="E65" s="4">
+        <v>5001</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G65" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" s="4">
+        <v>100401</v>
+      </c>
+      <c r="C66" s="4">
+        <v>5000</v>
+      </c>
+      <c r="D66" s="4">
+        <v>10040104</v>
+      </c>
+      <c r="E66" s="4">
+        <v>5001</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G66" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67" s="4">
+        <v>100401</v>
+      </c>
+      <c r="C67" s="4">
+        <v>5000</v>
+      </c>
+      <c r="D67" s="4">
+        <v>10040105</v>
+      </c>
+      <c r="E67" s="4">
+        <v>5001</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G67" s="4">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3411,11 +3692,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I75"/>
+  <dimension ref="B1:I83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F70" sqref="F70:F75"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B77" sqref="B77:H80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5106,6 +5387,170 @@
         <v>1</v>
       </c>
     </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B77" s="2">
+        <v>1</v>
+      </c>
+      <c r="C77" s="2">
+        <v>10</v>
+      </c>
+      <c r="D77" s="2">
+        <v>1</v>
+      </c>
+      <c r="E77" s="2">
+        <v>5000</v>
+      </c>
+      <c r="F77" s="2">
+        <v>1004</v>
+      </c>
+      <c r="G77" s="2">
+        <v>0</v>
+      </c>
+      <c r="H77" s="2">
+        <v>1</v>
+      </c>
+      <c r="I77" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B78" s="2">
+        <v>1</v>
+      </c>
+      <c r="C78" s="2">
+        <v>10</v>
+      </c>
+      <c r="D78" s="2">
+        <v>1</v>
+      </c>
+      <c r="E78" s="2">
+        <v>5000</v>
+      </c>
+      <c r="F78" s="2">
+        <v>100401</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79">
+        <v>5001</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>5001</v>
+      </c>
+      <c r="F79">
+        <v>10040101</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>1</v>
+      </c>
+      <c r="C80">
+        <v>5001</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="E80">
+        <v>5001</v>
+      </c>
+      <c r="F80">
+        <v>10040102</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="4">
+        <v>1</v>
+      </c>
+      <c r="C81" s="4">
+        <v>5001</v>
+      </c>
+      <c r="D81" s="4">
+        <v>1</v>
+      </c>
+      <c r="E81" s="4">
+        <v>5001</v>
+      </c>
+      <c r="F81" s="4">
+        <v>10040103</v>
+      </c>
+      <c r="G81" s="4">
+        <v>0</v>
+      </c>
+      <c r="H81" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B82" s="4">
+        <v>1</v>
+      </c>
+      <c r="C82" s="4">
+        <v>5001</v>
+      </c>
+      <c r="D82" s="4">
+        <v>1</v>
+      </c>
+      <c r="E82" s="4">
+        <v>5001</v>
+      </c>
+      <c r="F82" s="4">
+        <v>10040104</v>
+      </c>
+      <c r="G82" s="4">
+        <v>0</v>
+      </c>
+      <c r="H82" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B83" s="4">
+        <v>1</v>
+      </c>
+      <c r="C83" s="4">
+        <v>5001</v>
+      </c>
+      <c r="D83" s="4">
+        <v>1</v>
+      </c>
+      <c r="E83" s="4">
+        <v>5001</v>
+      </c>
+      <c r="F83" s="4">
+        <v>10040105</v>
+      </c>
+      <c r="G83" s="4">
+        <v>0</v>
+      </c>
+      <c r="H83" s="4">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>